<commit_message>
latest changes on the plane!
</commit_message>
<xml_diff>
--- a/1_visualization/9_application/data/gross_energy_production_original.xlsx
+++ b/1_visualization/9_application/data/gross_energy_production_original.xlsx
@@ -5,25 +5,40 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandres/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastiandres/Projects/europycon/europython_workshop_activities/1_visualization/9_application/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB005F28-C3AB-CE42-BC66-E7329C108407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A55BBC-1156-1E49-B2AC-0244DD21D437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - net_consumption_energ" sheetId="1" r:id="rId1"/>
+    <sheet name="gross_electricity_production" sheetId="1" r:id="rId1"/>
+    <sheet name="total_yearly" sheetId="3" r:id="rId2"/>
+    <sheet name="2023" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1 - net_consumption_energ'!$A$1:$E$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">gross_electricity_production!$A$1:$E$71</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="23">
   <si>
     <t>indicator</t>
   </si>
@@ -72,16 +87,40 @@
   <si>
     <t>nuclear</t>
   </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Gross Production Per capita</t>
+  </si>
+  <si>
+    <t>Gross Production Per capita per hour</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -89,6 +128,24 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -115,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -228,13 +285,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -280,9 +365,41 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1412,8 +1529,8 @@
   </sheetPr>
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2646,4 +2763,464 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43340C46-AA5D-7F4A-BFB1-28808C8A7E7D}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+      <c r="A1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="15">
+        <v>2010</v>
+      </c>
+      <c r="B2" s="17">
+        <v>85903</v>
+      </c>
+      <c r="C2" s="18">
+        <v>10000000</v>
+      </c>
+      <c r="D2" s="17">
+        <f>B2*1000000000/C2</f>
+        <v>8590300</v>
+      </c>
+      <c r="E2" s="17">
+        <f>D2/(365.25*24)</f>
+        <v>979.95665069587039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="15">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="17">
+        <v>87477</v>
+      </c>
+      <c r="C3" s="18">
+        <v>10000001</v>
+      </c>
+      <c r="D3" s="17">
+        <f t="shared" ref="D3:D15" si="0">B3*1000000000/C3</f>
+        <v>8747699.125230087</v>
+      </c>
+      <c r="E3" s="17">
+        <f t="shared" ref="E3:E15" si="1">D3/(365.25*24)</f>
+        <v>997.91228898358281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="15">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="17">
+        <v>87418</v>
+      </c>
+      <c r="C4" s="18">
+        <v>10000002</v>
+      </c>
+      <c r="D4" s="17">
+        <f t="shared" si="0"/>
+        <v>8741798.2516403496</v>
+      </c>
+      <c r="E4" s="17">
+        <f t="shared" si="1"/>
+        <v>997.23913434181497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="15">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="17">
+        <v>86913</v>
+      </c>
+      <c r="C5" s="18">
+        <v>10000003</v>
+      </c>
+      <c r="D5" s="17">
+        <f t="shared" si="0"/>
+        <v>8691297.3926107828</v>
+      </c>
+      <c r="E5" s="17">
+        <f t="shared" si="1"/>
+        <v>991.47814198160881</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="15">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="17">
+        <v>86148</v>
+      </c>
+      <c r="C6" s="18">
+        <v>10000004</v>
+      </c>
+      <c r="D6" s="17">
+        <f t="shared" si="0"/>
+        <v>8614796.5540813785</v>
+      </c>
+      <c r="E6" s="17">
+        <f t="shared" si="1"/>
+        <v>982.75114694060903</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="15">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="17">
+        <v>83892</v>
+      </c>
+      <c r="C7" s="18">
+        <v>10000005</v>
+      </c>
+      <c r="D7" s="17">
+        <f t="shared" si="0"/>
+        <v>8389195.8054020982</v>
+      </c>
+      <c r="E7" s="17">
+        <f t="shared" si="1"/>
+        <v>957.0152641343941</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="15">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="17">
+        <v>83309</v>
+      </c>
+      <c r="C8" s="18">
+        <v>10000006</v>
+      </c>
+      <c r="D8" s="17">
+        <f t="shared" si="0"/>
+        <v>8330895.0014629988</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="1"/>
+        <v>950.36447655293159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="15">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="17">
+        <v>87050</v>
+      </c>
+      <c r="C9" s="18">
+        <v>10000007</v>
+      </c>
+      <c r="D9" s="17">
+        <f t="shared" si="0"/>
+        <v>8704993.906504266</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" si="1"/>
+        <v>993.0406007876187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="15">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="17">
+        <v>88032</v>
+      </c>
+      <c r="C10" s="18">
+        <v>10000008</v>
+      </c>
+      <c r="D10" s="17">
+        <f t="shared" si="0"/>
+        <v>8803192.9574456345</v>
+      </c>
+      <c r="E10" s="17">
+        <f t="shared" si="1"/>
+        <v>1004.2428653257625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="15">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="17">
+        <v>87031</v>
+      </c>
+      <c r="C11" s="18">
+        <v>10000009</v>
+      </c>
+      <c r="D11" s="17">
+        <f t="shared" si="0"/>
+        <v>8703092.1672170497</v>
+      </c>
+      <c r="E11" s="17">
+        <f t="shared" si="1"/>
+        <v>992.82365585410105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="15">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="17">
+        <v>81517</v>
+      </c>
+      <c r="C12" s="18">
+        <v>10000010</v>
+      </c>
+      <c r="D12" s="17">
+        <f t="shared" si="0"/>
+        <v>8151691.8483081516</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" si="1"/>
+        <v>929.92149763953364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="15">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="17">
+        <v>85016</v>
+      </c>
+      <c r="C13" s="18">
+        <v>10000011</v>
+      </c>
+      <c r="D13" s="17">
+        <f t="shared" si="0"/>
+        <v>8501590.6482502874</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" si="1"/>
+        <v>969.83694367445673</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="15">
+        <v>2022</v>
+      </c>
+      <c r="B14" s="17">
+        <v>84848.14</v>
+      </c>
+      <c r="C14" s="18">
+        <v>10000012</v>
+      </c>
+      <c r="D14" s="17">
+        <f t="shared" si="0"/>
+        <v>8484803.8182354178</v>
+      </c>
+      <c r="E14" s="17">
+        <f t="shared" si="1"/>
+        <v>967.92195051738736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="15">
+        <v>2023</v>
+      </c>
+      <c r="B15" s="17">
+        <v>77245.787000000011</v>
+      </c>
+      <c r="C15" s="18">
+        <v>10000013</v>
+      </c>
+      <c r="D15" s="17">
+        <f t="shared" si="0"/>
+        <v>7724568.6580607463</v>
+      </c>
+      <c r="E15" s="17">
+        <f t="shared" si="1"/>
+        <v>881.19651586364887</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3F55B3-93FD-0A42-B525-5B6E750D0D92}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="20">
+        <v>39506.288</v>
+      </c>
+      <c r="F2" s="23">
+        <f>E2/$E$7</f>
+        <v>0.51143615120394847</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2023</v>
+      </c>
+      <c r="E3" s="21">
+        <v>30410.464</v>
+      </c>
+      <c r="F3" s="23">
+        <f>E3/$E$7</f>
+        <v>0.39368443485468013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2023</v>
+      </c>
+      <c r="E4" s="21">
+        <v>3416.9969999999998</v>
+      </c>
+      <c r="F4" s="23">
+        <f>E4/$E$7</f>
+        <v>4.4235383348479568E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2023</v>
+      </c>
+      <c r="E5" s="21">
+        <v>3210.4319999999998</v>
+      </c>
+      <c r="F5" s="23">
+        <f>E5/$E$7</f>
+        <v>4.1561256926542792E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2023</v>
+      </c>
+      <c r="E6" s="21">
+        <v>701.60599999999999</v>
+      </c>
+      <c r="F6" s="23">
+        <f>E6/$E$7</f>
+        <v>9.0827736663489471E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="D7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="24">
+        <f>SUM(E2:E6)</f>
+        <v>77245.787000000011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>